<commit_message>
Fixed "object null exception"
</commit_message>
<xml_diff>
--- a/ExcelMvc/ExcelMvc/Sample.Views/Forbes2000.xlsx
+++ b/ExcelMvc/ExcelMvc/Sample.Views/Forbes2000.xlsx
@@ -1194,8 +1194,8 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>4752975</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1205,7 +1205,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5067300" y="6991350"/>
-          <a:ext cx="7581900" cy="2105025"/>
+          <a:ext cx="7581900" cy="2352675"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1249,7 +1249,31 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>ExcelMvc  tables/fors view must be defined within ranges named in the format of</a:t>
+            <a:t>ExcelMvc  tables</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> and </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>forms must be defined within ranges named in the format of</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-AU" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
@@ -1297,7 +1321,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>ExcelMvc.Form.XYZ. </a:t>
+            <a:t>ExcelMvc.Form.XYZ respectively. </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-AU" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
@@ -1309,7 +1333,31 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> They be can defined in anywhere in a workbook.  See ExcelMvc.Table.Company etc on the left.</a:t>
+            <a:t> They can be defined </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>anywhere</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> in  the workbook. </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1555,6 +1603,15 @@
             </a:rPr>
             <a:t> </a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-AU" sz="1100">
+            <a:solidFill>
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
           <a:endParaRPr lang="en-AU" sz="1100">
             <a:solidFill>
               <a:srgbClr val="C00000"/>
@@ -30698,8 +30755,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changed code to assume ExcelMVC command names are prefixed with "ExcelMvc.", e.g. "ExcelMvc.LoadFoebes".
Changed copyright notice
</commit_message>
<xml_diff>
--- a/ExcelMvc/ExcelMvc/Sample.Views/Forbes2000.xlsx
+++ b/ExcelMvc/ExcelMvc/Sample.Views/Forbes2000.xlsx
@@ -523,11 +523,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" checked="Checked" firstButton="1" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" firstButton="1" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
@@ -568,7 +568,7 @@
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="2" name="ShowDialog"/>
+          <xdr:cNvPr id="2" name="ExcelMvc.ShowDialog"/>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -619,7 +619,7 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="6" name="LoadForbes"/>
+          <xdr:cNvPr id="6" name="ExcelMvc.LoadForbes"/>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -666,7 +666,7 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="8" name="ClearForbes"/>
+          <xdr:cNvPr id="8" name="ExcelMvc.ClearForbes"/>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -724,7 +724,7 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="10" name="StartUpdate"/>
+          <xdr:cNvPr id="10" name="ExcelMvc.StartUpdate"/>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -775,7 +775,7 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="11" name="ShowColumn"/>
+          <xdr:cNvPr id="11" name="ExcelMvc.ShowColumn"/>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -1642,7 +1642,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="ShapeButton"/>
+        <xdr:cNvPr id="2" name="ExcelMvc.ShapeButton"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1705,7 +1705,7 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="4097" name="FormButton" hidden="1">
+            <xdr:cNvPr id="4097" name="ExcelMvc.FormButton" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4097"/>
@@ -1902,6 +1902,31 @@
           </a:r>
         </a:p>
         <a:p>
+          <a:endParaRPr lang="en-AU" sz="1100" b="1" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>All command names must be prefixed with "ExcelMvc.".</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
           <a:endParaRPr lang="en-AU" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -1925,7 +1950,7 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="4104" name="FormOptionButtonYes" hidden="1">
+            <xdr:cNvPr id="4104" name="ExcelMvc.FormOptionButtonYes" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4104"/>
@@ -1986,7 +2011,7 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="4105" name="FormOptionButtonNo" hidden="1">
+            <xdr:cNvPr id="4105" name="ExcelMvc.FormOptionButtonNo" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4105"/>
@@ -2047,7 +2072,7 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="4099" name="FormCheckBox" hidden="1">
+            <xdr:cNvPr id="4099" name="ExcelMvc.FormCheckBox" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4099"/>
@@ -2169,7 +2194,7 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="4109" name="FormOptionButtonMale" hidden="1">
+            <xdr:cNvPr id="4109" name="ExcelMvc.FormOptionButtonMale" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4109"/>
@@ -2230,7 +2255,7 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="4110" name="FormOptionButtonFemale" hidden="1">
+            <xdr:cNvPr id="4110" name="ExcelMvc.FormOptionButtonFemale" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4110"/>
@@ -2352,7 +2377,7 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="4112" name="FormListBox" hidden="1">
+            <xdr:cNvPr id="4112" name="ExcelMvc.FormListBox" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4112"/>
@@ -2393,7 +2418,7 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="4114" name="FormDropDown" hidden="1">
+            <xdr:cNvPr id="4114" name="ExcelMvc.FormDropDown" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4114"/>
@@ -2434,7 +2459,7 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="4115" name="FormSpinner" hidden="1">
+            <xdr:cNvPr id="4115" name="ExcelMvc.FormSpinner" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4115"/>
@@ -30755,8 +30780,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -31317,7 +31342,7 @@
   <dimension ref="H1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31391,7 +31416,7 @@
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="4097" r:id="rId4" name="FormButton">
+            <control shapeId="4097" r:id="rId4" name="ExcelMvc.FormButton">
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
@@ -31413,7 +31438,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="4099" r:id="rId5" name="FormCheckBox">
+            <control shapeId="4099" r:id="rId5" name="ExcelMvc.FormCheckBox">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -31435,7 +31460,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="4104" r:id="rId6" name="FormOptionButtonYes">
+            <control shapeId="4104" r:id="rId6" name="ExcelMvc.FormOptionButtonYes">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -31457,7 +31482,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="4105" r:id="rId7" name="FormOptionButtonNo">
+            <control shapeId="4105" r:id="rId7" name="ExcelMvc.FormOptionButtonNo">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -31501,7 +31526,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="4109" r:id="rId9" name="FormOptionButtonMale">
+            <control shapeId="4109" r:id="rId9" name="ExcelMvc.FormOptionButtonMale">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -31523,7 +31548,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="4110" r:id="rId10" name="FormOptionButtonFemale">
+            <control shapeId="4110" r:id="rId10" name="ExcelMvc.FormOptionButtonFemale">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -31567,7 +31592,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="4112" r:id="rId12" name="FormListBox">
+            <control shapeId="4112" r:id="rId12" name="ExcelMvc.FormListBox">
               <controlPr defaultSize="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -31589,7 +31614,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="4114" r:id="rId13" name="FormDropDown">
+            <control shapeId="4114" r:id="rId13" name="ExcelMvc.FormDropDown">
               <controlPr defaultSize="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -31611,7 +31636,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="4115" r:id="rId14" name="FormSpinner">
+            <control shapeId="4115" r:id="rId14" name="ExcelMvc.FormSpinner">
               <controlPr defaultSize="0" autoPict="0">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>

</xml_diff>

<commit_message>
Refactored Sample.Application.ViewModel.Forbes.cs and moved common logic to Sample.Application.ViewModel.Forbes2000.cs
</commit_message>
<xml_diff>
--- a/ExcelMvc/ExcelMvc/Sample.Views/Forbes2000.xlsx
+++ b/ExcelMvc/ExcelMvc/Sample.Views/Forbes2000.xlsx
@@ -567,7 +567,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -860,7 +860,7 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="11" name="ExcelMvc.ShowColumn"/>
+          <xdr:cNvPr id="11" name="ExcelMvc.ShowIndustry"/>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -1492,7 +1492,7 @@
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="4" name="ExcelMvc.TransposedShowDialog"/>
+          <xdr:cNvPr id="4" name="ExcelMvc.ShowDialog"/>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -1543,7 +1543,7 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="5" name="ExcelMvc.TransposedLoadForbes"/>
+          <xdr:cNvPr id="5" name="ExcelMvc.LoadForbes"/>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -1590,7 +1590,7 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="6" name="ExcelMvc.TransposedClearForbes"/>
+          <xdr:cNvPr id="6" name="ExcelMvc.ClearForbes"/>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -1648,7 +1648,7 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="7" name="ExcelMvc.TransposedStartUpdate"/>
+          <xdr:cNvPr id="7" name="ExcelMvc.StartUpdate"/>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -1699,7 +1699,7 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="8" name="ExcelMvc.TransposedShowRow"/>
+          <xdr:cNvPr id="8" name="ExcelMvc.ShowIndustry"/>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -2401,7 +2401,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="de-DE" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-AU" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2646,7 +2646,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="de-DE" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-AU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2707,7 +2707,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="de-DE" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-AU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2768,7 +2768,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="de-DE" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-AU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2829,7 +2829,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="de-DE" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-AU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2890,7 +2890,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="de-DE" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-AU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -2951,7 +2951,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="de-DE" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-AU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3012,7 +3012,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="de-DE" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-AU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -3157,9 +3157,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3197,7 +3197,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -3269,7 +3269,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3448,10 +3448,10 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="B4:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="29" style="1" customWidth="1"/>
@@ -31417,10 +31417,10 @@
   <dimension ref="A5:CRZ30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" style="52" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" style="52"/>
@@ -54261,7 +54261,7 @@
       <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.7109375" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
@@ -54294,7 +54294,7 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.85546875" style="7" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" style="7" customWidth="1"/>
@@ -55292,7 +55292,7 @@
       <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
WIP:Company Filter Table as an example of One Way to Source binding, i.e. values in the table will be initialized to model objects.
</commit_message>
<xml_diff>
--- a/ExcelMvc/ExcelMvc/Sample.Views/Forbes2000.xlsx
+++ b/ExcelMvc/ExcelMvc/Sample.Views/Forbes2000.xlsx
@@ -18,6 +18,7 @@
     <definedName name="ExcelMvc.Form.Company">ExcelMvc!$A$35:$F$49</definedName>
     <definedName name="ExcelMvc.Form.CompanyTransposed">ExcelMvc!$A$54:$F$62</definedName>
     <definedName name="ExcelMvc.Table.Company">ExcelMvc!$A$2:$F$16</definedName>
+    <definedName name="ExcelMvc.Table.CompanyFilters">ExcelMvc!$A$76:$D$77</definedName>
     <definedName name="ExcelMvc.Table.CompanyTransposed">ExcelMvc!$A$21:$F$30</definedName>
     <definedName name="ExcelMvc.Table.Country">ExcelMvc!$A$67:$D$68</definedName>
     <definedName name="ExcelMvc.Table.Industry">ExcelMvc!$A$71:$D$72</definedName>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="52">
   <si>
     <t xml:space="preserve">Company </t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -181,6 +182,18 @@
   </si>
   <si>
     <t>ExcelMvc.Form.CompanyTransposed</t>
+  </si>
+  <si>
+    <t>ExcelMvc.Table.CompanyFilters</t>
+  </si>
+  <si>
+    <t>NameLike</t>
+  </si>
+  <si>
+    <t>(End of Company Filter table)</t>
+  </si>
+  <si>
+    <t>Company Filter  Tabele (NameLike)</t>
   </si>
 </sst>
 </file>
@@ -1762,16 +1775,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>28574</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1780,8 +1793,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4276724" y="114300"/>
-          <a:ext cx="5467351" cy="600075"/>
+          <a:off x="7067549" y="38100"/>
+          <a:ext cx="5467351" cy="1800225"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1825,7 +1838,31 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>These two tables will be loaded when "Load All" is  excuted. They are referenced from other tables as Excel validation lists</a:t>
+            <a:t>The Country Table</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> and Industry Table are </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>loaded  when  the "Load All" command is  excuted. They are referenced from other tables as Excel validation lists</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-AU" sz="1100" b="1" i="0" u="none" strike="noStrike">
@@ -1843,6 +1880,60 @@
             <a:rPr lang="en-AU"/>
             <a:t> </a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-AU"/>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100" b="1" i="0">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>The Country Filter Table</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100" b="1" i="0" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> is used to filter the companys in the Load All process. Use * to include all.  When the book is loaded,  the values in the table will be copied to the  CompanyFilter objects.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-AU">
+            <a:solidFill>
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
           <a:endParaRPr lang="en-AU" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -31417,7 +31508,7 @@
   <dimension ref="A5:CRZ30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -54255,16 +54346,17 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.7109375" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" customWidth="1"/>
     <col min="5" max="5" width="9.140625" customWidth="1"/>
     <col min="7" max="7" width="9.140625" customWidth="1"/>
   </cols>
@@ -54276,7 +54368,14 @@
       <c r="B1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="48"/>
+      <c r="C1" s="48" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" s="48" t="s">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -54290,8 +54389,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:L81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -55269,11 +55368,40 @@
       </c>
       <c r="D72" s="9"/>
     </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D76" s="10"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="12" t="str">
+        <f ca="1">CELL("address",References!C2)</f>
+        <v>[Forbes2000.xlsx]References!$C$2</v>
+      </c>
+      <c r="B77" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C77" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D77" s="9"/>
+    </row>
     <row r="81" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E81" s="8"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="G2:G5"/>
   </mergeCells>

</xml_diff>

<commit_message>
Added OneWayToSource form Settings. "UpdatedIntervalSeconds" is used to control real-time simulation speed.
</commit_message>
<xml_diff>
--- a/ExcelMvc/ExcelMvc/Sample.Views/Forbes2000.xlsx
+++ b/ExcelMvc/ExcelMvc/Sample.Views/Forbes2000.xlsx
@@ -17,6 +17,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Forbes!$B$5:$I$5</definedName>
     <definedName name="ExcelMvc.Form.Company">ExcelMvc!$A$35:$F$49</definedName>
     <definedName name="ExcelMvc.Form.CompanyTransposed">ExcelMvc!$A$54:$F$62</definedName>
+    <definedName name="ExcelMvc.Form.Settings">ExcelMvc!$A$80:$D$81</definedName>
     <definedName name="ExcelMvc.Table.Company">ExcelMvc!$A$2:$F$16</definedName>
     <definedName name="ExcelMvc.Table.CompanyFilters">ExcelMvc!$A$76:$D$77</definedName>
     <definedName name="ExcelMvc.Table.CompanyTransposed">ExcelMvc!$A$21:$F$30</definedName>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="57">
   <si>
     <t xml:space="preserve">Company </t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -190,16 +191,25 @@
     <t>NameLike</t>
   </si>
   <si>
-    <t>Company Filter  Tabele (NameLike)</t>
-  </si>
-  <si>
     <t>OneWayToSource</t>
   </si>
   <si>
     <t>*</t>
   </si>
   <si>
-    <t>(Specify up to 10 filters, * to load all)</t>
+    <t>(Specify up to 10 "OR" filters, * to load all)</t>
+  </si>
+  <si>
+    <t>Company Filter  Table (NameLike)</t>
+  </si>
+  <si>
+    <t>ExcelMvc.Form.Settings</t>
+  </si>
+  <si>
+    <t>UpdateIntervalSeconds</t>
+  </si>
+  <si>
+    <t>Update Interval Seconds</t>
   </si>
 </sst>
 </file>
@@ -646,8 +656,8 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>16236</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>231540</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
@@ -657,282 +667,364 @@
       <xdr:row>2</xdr:row>
       <xdr:rowOff>67556</xdr:rowOff>
     </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="3" name="Group 2"/>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
+    <xdr:sp macro="ExcelMvcRunCommandAction" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="ExcelMvc.ShowDialog"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5841765" y="104775"/>
+          <a:ext cx="1321034" cy="286631"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1200" b="1"/>
+            <a:t>Show</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1200" b="1" baseline="0"/>
+            <a:t> Dialog</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-AU" sz="1200" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>16236</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>549376</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>67556</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="ExcelMvcRunCommandAction" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="ExcelMvc.LoadForbes"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
         <a:xfrm>
           <a:off x="16236" y="104775"/>
-          <a:ext cx="7146563" cy="286631"/>
-          <a:chOff x="2911836" y="104775"/>
-          <a:chExt cx="7146563" cy="286631"/>
+          <a:ext cx="1314190" cy="286631"/>
         </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="2" name="ExcelMvc.ShowDialog"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="8737365" y="104775"/>
-            <a:ext cx="1321034" cy="286631"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="12700"/>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent6">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent6"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent6"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1200" b="1"/>
-              <a:t>Show</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1200" b="1" baseline="0"/>
-              <a:t> Dialog</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="en-AU" sz="1200" b="1"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="6" name="ExcelMvc.LoadForbes"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="2911836" y="104775"/>
-            <a:ext cx="1314190" cy="286631"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="12700"/>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent6">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent6"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent6"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1200" b="1"/>
-              <a:t>Load  Forbes 2000</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="en-AU" sz="1200" b="1"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="8" name="ExcelMvc.ClearForbes"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="4366508" y="104775"/>
-            <a:ext cx="1314190" cy="286631"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="12700"/>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent6">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent6"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent6"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1200" b="1"/>
-              <a:t>Clear</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1200" b="1" baseline="0"/>
-              <a:t> All</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="en-AU" sz="1200" b="1"/>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1200" b="1"/>
-              <a:t>C</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="10" name="ExcelMvc.StartUpdate"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="7275852" y="104775"/>
-            <a:ext cx="1321034" cy="286631"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="12700"/>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent6">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent6"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent6"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1200" b="1" baseline="0"/>
-              <a:t>Start  Update</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="en-AU" sz="1200" b="1" baseline="0"/>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="en-AU" sz="1200" b="1"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="11" name="ExcelMvc.ShowIndustry"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="5821180" y="104775"/>
-            <a:ext cx="1314190" cy="286631"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="12700"/>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent6">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent6"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent6"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1200" b="1"/>
-              <a:t>Hide Industry</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-AU" sz="1200" b="1" baseline="0"/>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="en-AU" sz="1200" b="1"/>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1200" b="1"/>
-              <a:t>C</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1200" b="1"/>
+            <a:t>Load  Forbes 2000</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-AU" sz="1200" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>689858</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>70473</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>67556</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="ExcelMvcRunCommandAction" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="ExcelMvc.ClearForbes"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1470908" y="104775"/>
+          <a:ext cx="1314190" cy="286631"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="90000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Clear</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1200" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="90000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> All</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-AU" sz="1200" b="1">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="90000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="90000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>C</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1665627</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>91061</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>67556</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="ExcelMvcRunCommandAction" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="ExcelMvc.StartUpdate"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4380252" y="104775"/>
+          <a:ext cx="1321034" cy="286631"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1200" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="90000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Start  Update</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-AU" sz="1200" b="1" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="90000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-AU" sz="1200" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>210955</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1525145</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>67556</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="ExcelMvcRunCommandAction" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="ExcelMvc.ShowIndustry"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2925580" y="104775"/>
+          <a:ext cx="1314190" cy="286631"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1200" b="1"/>
+            <a:t>Hide Industry</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-AU" sz="1200" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-AU" sz="1200" b="1"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1200" b="1"/>
+            <a:t>C</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
@@ -1485,8 +1577,8 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>62904</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
@@ -1496,282 +1588,364 @@
       <xdr:row>2</xdr:row>
       <xdr:rowOff>10406</xdr:rowOff>
     </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="3" name="Group 2"/>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
+    <xdr:sp macro="ExcelMvcRunCommandAction" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="ExcelMvc.ShowDialog"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5863629" y="104775"/>
+          <a:ext cx="1321034" cy="286631"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1200" b="1"/>
+            <a:t>Show</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1200" b="1" baseline="0"/>
+            <a:t> Dialog</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-AU" sz="1200" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>428365</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>10406</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="ExcelMvcRunCommandAction" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="ExcelMvc.LoadForbes"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
         <a:xfrm>
           <a:off x="38100" y="104775"/>
-          <a:ext cx="7146563" cy="286631"/>
-          <a:chOff x="2911836" y="104775"/>
-          <a:chExt cx="7146563" cy="286631"/>
+          <a:ext cx="1314190" cy="286631"/>
         </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="4" name="ExcelMvc.ShowDialog"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="8737365" y="104775"/>
-            <a:ext cx="1321034" cy="286631"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="12700"/>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent6">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent6"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent6"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1200" b="1"/>
-              <a:t>Show</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1200" b="1" baseline="0"/>
-              <a:t> Dialog</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="en-AU" sz="1200" b="1"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="5" name="ExcelMvc.LoadForbes"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="2911836" y="104775"/>
-            <a:ext cx="1314190" cy="286631"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="12700"/>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent6">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent6"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent6"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1200" b="1"/>
-              <a:t>Load  Forbes 2000</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="en-AU" sz="1200" b="1"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="6" name="ExcelMvc.ClearForbes"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="4366508" y="104775"/>
-            <a:ext cx="1314190" cy="286631"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="12700"/>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent6">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent6"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent6"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1200" b="1"/>
-              <a:t>Clear</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1200" b="1" baseline="0"/>
-              <a:t> All</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="en-AU" sz="1200" b="1"/>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1200" b="1"/>
-              <a:t>C</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="7" name="ExcelMvc.StartUpdate"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="7275852" y="104775"/>
-            <a:ext cx="1321034" cy="286631"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="12700"/>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent6">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent6"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent6"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1200" b="1" baseline="0"/>
-              <a:t>Start  Update</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="en-AU" sz="1200" b="1" baseline="0"/>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="en-AU" sz="1200" b="1"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="8" name="ExcelMvc.ShowIndustry"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="5821180" y="104775"/>
-            <a:ext cx="1314190" cy="286631"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="12700"/>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent6">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent6"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent6"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1200" b="1"/>
-              <a:t>Hide Industry</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-AU" sz="1200" b="1" baseline="0"/>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="en-AU" sz="1200" b="1"/>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1200" b="1"/>
-              <a:t>C</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1200" b="1"/>
+            <a:t>Load  Forbes 2000</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-AU" sz="1200" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>568847</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>130437</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>10406</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="ExcelMvcRunCommandAction" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="ExcelMvc.ClearForbes"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1492772" y="104775"/>
+          <a:ext cx="1314190" cy="286631"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="90000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Clear</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1200" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="90000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> All</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-AU" sz="1200" b="1">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="90000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="90000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>C</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>125391</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>684425</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>10406</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="ExcelMvcRunCommandAction" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="ExcelMvc.StartUpdate"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4402116" y="104775"/>
+          <a:ext cx="1321034" cy="286631"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1200" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="90000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Start  Update</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-AU" sz="1200" b="1" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="90000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-AU" sz="1200" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>270919</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1585109</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>10406</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="ExcelMvcRunCommandAction" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="ExcelMvc.ShowIndustry"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2947444" y="104775"/>
+          <a:ext cx="1314190" cy="286631"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1200" b="1"/>
+            <a:t>Hide Industry</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-AU" sz="1200" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-AU" sz="1200" b="1"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1200" b="1"/>
+            <a:t>C</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1844,7 +2018,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>The Country Table</a:t>
+            <a:t>The Country table</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-AU" sz="1100" b="1" i="0" u="none" strike="noStrike" baseline="0">
@@ -1856,7 +2030,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> and Industry Table are </a:t>
+            <a:t> and Industry table are </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-AU" sz="1100" b="1" i="0" u="none" strike="noStrike">
@@ -1918,7 +2092,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>The Country Filter Table</a:t>
+            <a:t>The Country Filter table</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-AU" sz="1100" b="1" i="0" baseline="0">
@@ -1931,6 +2105,65 @@
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t> is used to filter the companys in the Load All process. Use * to include all.  When the book is loaded,  the values in the table will be copied to the  CompanyFilter objects.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-AU" sz="1100" b="1" i="0" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100" b="1" i="0" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>The Settings  form specifies  application settings. Only Update Interval Seconds is demostrated here.</a:t>
           </a:r>
           <a:endParaRPr lang="en-AU">
             <a:solidFill>
@@ -2407,7 +2640,7 @@
       <xdr:row>2</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp macro="ExcelMvcRunCommandAction" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="ExcelMvc.ShapeButton"/>
         <xdr:cNvSpPr/>
@@ -3545,7 +3778,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -54352,22 +54585,22 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.7109375" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="3" max="3" width="32.85546875" customWidth="1"/>
+    <col min="3" max="3" width="37.85546875" customWidth="1"/>
     <col min="5" max="5" width="9.140625" customWidth="1"/>
     <col min="7" max="7" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>12</v>
       </c>
@@ -54375,17 +54608,25 @@
         <v>13</v>
       </c>
       <c r="C1" s="48" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="48" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C12" s="48" t="s">
-        <v>53</v>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14" s="48" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -54400,14 +54641,14 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:L81"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.85546875" style="7" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="7" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" style="7" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" style="7" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="45" style="7" customWidth="1"/>
@@ -55405,11 +55646,39 @@
         <v>49</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D77" s="9"/>
     </row>
-    <row r="81" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D80" s="10"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="12" t="str">
+        <f ca="1">CELL("address",References!D14)</f>
+        <v>[Forbes2000.xlsx]References!$D$14</v>
+      </c>
+      <c r="B81" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C81" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D81" s="9"/>
       <c r="E81" s="8"/>
     </row>
   </sheetData>
@@ -55503,7 +55772,7 @@
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
             <control shapeId="4097" r:id="rId4" name="ExcelMvc.FormButton">
-              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="ExcelMvcRunCommandAction">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
@@ -55525,7 +55794,7 @@
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
             <control shapeId="4099" r:id="rId5" name="ExcelMvc.FormCheckBox">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" macro="ExcelMvcRunCommandAction">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
@@ -55547,7 +55816,7 @@
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
             <control shapeId="4104" r:id="rId6" name="ExcelMvc.FormOptionButtonYes">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" macro="ExcelMvcRunCommandAction">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
@@ -55569,7 +55838,7 @@
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
             <control shapeId="4105" r:id="rId7" name="ExcelMvc.FormOptionButtonNo">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" macro="ExcelMvcRunCommandAction">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
@@ -55613,7 +55882,7 @@
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
             <control shapeId="4109" r:id="rId9" name="ExcelMvc.FormOptionButtonMale">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" macro="ExcelMvcRunCommandAction">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
@@ -55635,7 +55904,7 @@
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
             <control shapeId="4110" r:id="rId10" name="ExcelMvc.FormOptionButtonFemale">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" macro="ExcelMvcRunCommandAction">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
@@ -55679,7 +55948,7 @@
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
             <control shapeId="4112" r:id="rId12" name="ExcelMvc.FormListBox">
-              <controlPr defaultSize="0" autoLine="0" autoPict="0">
+              <controlPr defaultSize="0" autoLine="0" autoPict="0" macro="ExcelMvcRunCommandAction">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>3</xdr:col>
@@ -55701,7 +55970,7 @@
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
             <control shapeId="4114" r:id="rId13" name="ExcelMvc.FormDropDown">
-              <controlPr defaultSize="0" autoLine="0" autoPict="0">
+              <controlPr defaultSize="0" autoLine="0" autoPict="0" macro="ExcelMvcRunCommandAction">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>3</xdr:col>
@@ -55723,7 +55992,7 @@
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
             <control shapeId="4115" r:id="rId14" name="ExcelMvc.FormSpinner">
-              <controlPr defaultSize="0" autoPict="0">
+              <controlPr defaultSize="0" autoPict="0" macro="ExcelMvcRunCommandAction">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
                     <xdr:col>3</xdr:col>

</xml_diff>